<commit_message>
Loot Table Test & Added Drop Book
</commit_message>
<xml_diff>
--- a/item_number.xlsx
+++ b/item_number.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
   <si>
     <t xml:space="preserve">Base Item</t>
   </si>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t xml:space="preserve">곧 파란색 책으로 텍스트 교체 예정.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enchanted_book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drop_book</t>
   </si>
 </sst>
 </file>
@@ -292,6 +298,7 @@
       <sz val="10"/>
       <name val="나눔고딕"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -376,7 +383,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
+      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -983,6 +990,12 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>87</v>
+      </c>
       <c r="C52" s="0" t="n">
         <v>700051</v>
       </c>

</xml_diff>

<commit_message>
Added TwoHand Skill & Axe Skills & Added Undead Predicate
</commit_message>
<xml_diff>
--- a/item_number.xlsx
+++ b/item_number.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChanW\AppData\Roaming\.minecraft\saves\Arc_Mode\datapacks\arc-mode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCServer\world\datapacks\arc-mode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBD9C34-83A2-46F7-A3A7-70E6AF7044BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38837C37-73E3-489B-83AB-42B19E3B36D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="A12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -842,13 +842,13 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>700011</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Item & Mob registering
</commit_message>
<xml_diff>
--- a/item_number.xlsx
+++ b/item_number.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCServer\world\datapacks\arc-mode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DB45C5-ED9A-430B-98A4-E532FE072880}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBB9024-E3FA-4DDE-9B86-2724656255E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="95">
   <si>
     <t>Base Item</t>
   </si>
@@ -310,12 +310,40 @@
     <t>stick</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>panda_spawn_egg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cryob/core</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cat_spawn_egg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cryob/elder_guardian_eye</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔더의 눈 텍스쳐 덮어씌우셈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blaze_spawn_egg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cryob/guardian_eye</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="나눔고딕"/>
@@ -337,6 +365,12 @@
     <font>
       <sz val="10"/>
       <name val="나눔고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="굴림"/>
       <family val="2"/>
       <charset val="129"/>
     </font>
@@ -367,12 +401,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -687,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C46" sqref="A46:C47"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -1296,7 +1331,43 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="13.5">
-      <c r="A53" s="3"/>
+      <c r="A53" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="2">
+        <v>700052</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="13.5">
+      <c r="A54" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="2">
+        <v>700053</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="2">
+        <v>700054</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Loot Table Added & Updated Hammer Skill & Added Loots
</commit_message>
<xml_diff>
--- a/item_number.xlsx
+++ b/item_number.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCServer\world\datapacks\arc-mode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBB9024-E3FA-4DDE-9B86-2724656255E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E157BEB-5387-43CA-9A7D-AC286E0EFE7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="255" windowWidth="16695" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>platinum/platinum_warhammer</t>
-  </si>
-  <si>
-    <t>bee_spawn_egg</t>
   </si>
   <si>
     <t>jungle/illusion_soul</t>
@@ -336,6 +333,10 @@
   </si>
   <si>
     <t>cryob/guardian_eye</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drowned_spawn_egg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -724,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -742,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -773,7 +774,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="2">
         <v>700002</v>
@@ -945,12 +946,12 @@
         <v>700016</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:5" ht="13.5">
+      <c r="A18" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C18" s="2">
         <v>700017</v>
@@ -961,7 +962,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2">
         <v>700018</v>
@@ -969,19 +970,19 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C20" s="2">
         <v>700019</v>
       </c>
       <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
         <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -989,7 +990,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2">
         <v>700020</v>
@@ -997,42 +998,42 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C22" s="2">
         <v>700021</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -1041,7 +1042,7 @@
         <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="2">
         <v>700025</v>
@@ -1049,10 +1050,10 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C27" s="2">
         <v>700026</v>
@@ -1060,10 +1061,10 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C28" s="2">
         <v>700027</v>
@@ -1074,7 +1075,7 @@
         <v>19</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="2">
         <v>700028</v>
@@ -1085,7 +1086,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="2">
         <v>700029</v>
@@ -1096,7 +1097,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="2">
         <v>700030</v>
@@ -1107,7 +1108,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="2">
         <v>700031</v>
@@ -1118,7 +1119,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="2">
         <v>700032</v>
@@ -1126,10 +1127,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="2">
         <v>700033</v>
@@ -1137,28 +1138,28 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="2"/>
     </row>
@@ -1167,7 +1168,7 @@
         <v>21</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" s="2">
         <v>700037</v>
@@ -1178,7 +1179,7 @@
         <v>19</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C39" s="2">
         <v>700038</v>
@@ -1186,10 +1187,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="C40" s="2">
         <v>700039</v>
@@ -1197,10 +1198,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C41" s="2">
         <v>700040</v>
@@ -1208,10 +1209,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C42" s="2">
         <v>700041</v>
@@ -1219,10 +1220,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C43" s="2">
         <v>700042</v>
@@ -1230,10 +1231,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="C44" s="2">
         <v>700043</v>
@@ -1241,10 +1242,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" s="2">
         <v>700044</v>
@@ -1252,10 +1253,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="C46" s="2">
         <v>700045</v>
@@ -1263,10 +1264,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C47" s="2">
         <v>700046</v>
@@ -1274,10 +1275,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C48" s="2">
         <v>700047</v>
@@ -1288,7 +1289,7 @@
         <v>4</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C49" s="2">
         <v>700048</v>
@@ -1296,10 +1297,10 @@
     </row>
     <row r="50" spans="1:4" ht="13.5">
       <c r="A50" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C50" s="2">
         <v>700049</v>
@@ -1307,24 +1308,24 @@
     </row>
     <row r="51" spans="1:4" ht="13.5">
       <c r="A51" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C51" s="2">
         <v>700034</v>
       </c>
       <c r="D51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C52" s="2">
         <v>700051</v>
@@ -1332,10 +1333,10 @@
     </row>
     <row r="53" spans="1:4" ht="13.5">
       <c r="A53" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="C53" s="2">
         <v>700052</v>
@@ -1343,30 +1344,30 @@
     </row>
     <row r="54" spans="1:4" ht="13.5">
       <c r="A54" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C54" s="2">
         <v>700053</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C55" s="2">
         <v>700054</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix & bow added & made coin & made enchantment fully
</commit_message>
<xml_diff>
--- a/item_number.xlsx
+++ b/item_number.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCServer\world\datapacks\arc-mode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FEE6F2-0B34-4E65-AD60-157CAA4F27FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0F9115-BE9E-46B9-B06B-0F497368BFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="255" windowWidth="16695" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="113">
   <si>
     <t>Base Item</t>
   </si>
@@ -276,27 +276,6 @@
     <t>drop_book</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>write with +</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="나눔고딕"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> item/custom/</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>broken/broken_crystal_saber</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -338,6 +317,82 @@
   </si>
   <si>
     <t>evoker_spawn_egg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bread</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>potion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron_ingot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gold_nugget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin/copper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>write with + item/custom/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin/iron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin/diamond</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin/netherite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>netherite_ingot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diamond</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diamond_axe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkknight/darkknight_axe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diamond_shovel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkknight/darkknight_onehand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diamond_hoe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkknight/darkknight_scythe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mineshaft/light_bow</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -345,7 +400,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <name val="나눔고딕"/>
@@ -361,20 +416,9 @@
     <font>
       <sz val="10"/>
       <name val="맑은 고딕"/>
-      <family val="2"/>
+      <family val="3"/>
       <charset val="129"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="나눔고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="굴림"/>
-      <family val="2"/>
-      <charset val="129"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -403,13 +447,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -724,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -739,24 +781,25 @@
     <col min="5" max="1025" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="13.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="13.5">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -766,25 +809,29 @@
       <c r="C2" s="2">
         <v>700001</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2">
         <v>700002</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="13.5">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -794,11 +841,13 @@
       <c r="C4" s="2">
         <v>700003</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="13.5">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -808,11 +857,13 @@
       <c r="C5" s="2">
         <v>700004</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="13.5">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -822,11 +873,13 @@
       <c r="C6" s="2">
         <v>700005</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="13.5">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -836,8 +889,11 @@
       <c r="C7" s="2">
         <v>700006</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="13.5">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -847,8 +903,11 @@
       <c r="C8" s="2">
         <v>700007</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="13.5">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -858,8 +917,11 @@
       <c r="C9" s="2">
         <v>700008</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="13.5">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -869,8 +931,11 @@
       <c r="C10" s="2">
         <v>700009</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="13.5">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -880,8 +945,11 @@
       <c r="C11" s="2">
         <v>700010</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="13.5">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -891,8 +959,11 @@
       <c r="C12" s="2">
         <v>700011</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="13.5">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -902,8 +973,11 @@
       <c r="C13" s="2">
         <v>700012</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="13.5">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -913,8 +987,11 @@
       <c r="C14" s="2">
         <v>700013</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="13.5">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -924,8 +1001,11 @@
       <c r="C15" s="2">
         <v>700014</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="13.5">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -935,8 +1015,11 @@
       <c r="C16" s="2">
         <v>700015</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="13.5">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -946,10 +1029,13 @@
       <c r="C17" s="2">
         <v>700016</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="13.5">
-      <c r="A18" s="4" t="s">
-        <v>93</v>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="13.5">
+      <c r="A18" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>34</v>
@@ -957,8 +1043,11 @@
       <c r="C18" s="2">
         <v>700017</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="13.5">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -968,8 +1057,11 @@
       <c r="C19" s="2">
         <v>700018</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" ht="13.5">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -979,14 +1071,15 @@
       <c r="C20" s="2">
         <v>700019</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" ht="13.5">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -996,8 +1089,11 @@
       <c r="C21" s="2">
         <v>700020</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" ht="13.5">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
@@ -1007,11 +1103,13 @@
       <c r="C22" s="2">
         <v>700021</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="13.5">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -1019,8 +1117,11 @@
         <v>44</v>
       </c>
       <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" ht="13.5">
       <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
@@ -1028,8 +1129,11 @@
         <v>45</v>
       </c>
       <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" ht="13.5">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1037,8 +1141,11 @@
         <v>46</v>
       </c>
       <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="13.5">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1048,8 +1155,11 @@
       <c r="C26" s="2">
         <v>700025</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="13.5">
       <c r="A27" s="2" t="s">
         <v>48</v>
       </c>
@@ -1059,8 +1169,11 @@
       <c r="C27" s="2">
         <v>700026</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" ht="13.5">
       <c r="A28" s="2" t="s">
         <v>50</v>
       </c>
@@ -1070,8 +1183,11 @@
       <c r="C28" s="2">
         <v>700027</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" ht="13.5">
       <c r="A29" s="2" t="s">
         <v>19</v>
       </c>
@@ -1081,8 +1197,11 @@
       <c r="C29" s="2">
         <v>700028</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" ht="13.5">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -1092,8 +1211,11 @@
       <c r="C30" s="2">
         <v>700029</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" ht="13.5">
       <c r="A31" s="2" t="s">
         <v>23</v>
       </c>
@@ -1103,8 +1225,11 @@
       <c r="C31" s="2">
         <v>700030</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" ht="13.5">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1114,8 +1239,11 @@
       <c r="C32" s="2">
         <v>700031</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" ht="13.5">
       <c r="A33" s="2" t="s">
         <v>19</v>
       </c>
@@ -1125,8 +1253,11 @@
       <c r="C33" s="2">
         <v>700032</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" ht="13.5">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
@@ -1136,8 +1267,11 @@
       <c r="C34" s="2">
         <v>700033</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" ht="13.5">
       <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
@@ -1145,8 +1279,11 @@
         <v>58</v>
       </c>
       <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" ht="13.5">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1154,8 +1291,11 @@
         <v>59</v>
       </c>
       <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" ht="13.5">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1163,8 +1303,11 @@
         <v>60</v>
       </c>
       <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" ht="13.5">
       <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
@@ -1174,8 +1317,11 @@
       <c r="C38" s="2">
         <v>700037</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" ht="13.5">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -1185,10 +1331,13 @@
       <c r="C39" s="2">
         <v>700038</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="13.5">
-      <c r="A40" s="4" t="s">
-        <v>94</v>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" ht="13.5">
+      <c r="A40" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>63</v>
@@ -1196,8 +1345,11 @@
       <c r="C40" s="2">
         <v>700039</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" ht="13.5">
       <c r="A41" s="2" t="s">
         <v>64</v>
       </c>
@@ -1207,8 +1359,11 @@
       <c r="C41" s="2">
         <v>700040</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" ht="13.5">
       <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
@@ -1218,8 +1373,11 @@
       <c r="C42" s="2">
         <v>700041</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" ht="13.5">
       <c r="A43" s="2" t="s">
         <v>68</v>
       </c>
@@ -1229,8 +1387,11 @@
       <c r="C43" s="2">
         <v>700042</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" ht="13.5">
       <c r="A44" s="2" t="s">
         <v>70</v>
       </c>
@@ -1240,8 +1401,11 @@
       <c r="C44" s="2">
         <v>700043</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" ht="13.5">
       <c r="A45" s="2" t="s">
         <v>68</v>
       </c>
@@ -1251,8 +1415,11 @@
       <c r="C45" s="2">
         <v>700044</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" ht="13.5">
       <c r="A46" s="2" t="s">
         <v>73</v>
       </c>
@@ -1262,8 +1429,11 @@
       <c r="C46" s="2">
         <v>700045</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" ht="13.5">
       <c r="A47" s="2" t="s">
         <v>73</v>
       </c>
@@ -1273,8 +1443,11 @@
       <c r="C47" s="2">
         <v>700046</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" ht="13.5">
       <c r="A48" s="2" t="s">
         <v>64</v>
       </c>
@@ -1284,8 +1457,11 @@
       <c r="C48" s="2">
         <v>700047</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" ht="13.5">
       <c r="A49" s="2" t="s">
         <v>4</v>
       </c>
@@ -1295,10 +1471,13 @@
       <c r="C49" s="2">
         <v>700048</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="13.5">
-      <c r="A50" s="4" t="s">
-        <v>85</v>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" ht="13.5">
+      <c r="A50" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>78</v>
@@ -1306,10 +1485,13 @@
       <c r="C50" s="2">
         <v>700049</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="13.5">
-      <c r="A51" s="4" t="s">
-        <v>85</v>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" ht="13.5">
+      <c r="A51" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>79</v>
@@ -1317,11 +1499,13 @@
       <c r="C51" s="2">
         <v>700034</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" ht="13.5">
       <c r="A52" s="2" t="s">
         <v>81</v>
       </c>
@@ -1331,45 +1515,291 @@
       <c r="C52" s="2">
         <v>700051</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="13.5">
-      <c r="A53" s="3" t="s">
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" ht="13.5">
+      <c r="A53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="C53" s="2">
         <v>700052</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="13.5">
-      <c r="A54" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>92</v>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" ht="13.5">
+      <c r="A54" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="C54" s="2">
         <v>700053</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" ht="13.5">
+      <c r="A55" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>89</v>
+      <c r="B55" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="C55" s="2">
         <v>700054</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>90</v>
-      </c>
+      <c r="D55" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" ht="13.5">
+      <c r="A56" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="2">
+        <v>700055</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" ht="13.5">
+      <c r="A57" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="3">
+        <v>700056</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" ht="13.5">
+      <c r="A58" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="3">
+        <v>700057</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" ht="13.5">
+      <c r="A59" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="3">
+        <v>700058</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" ht="13.5">
+      <c r="A60" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" s="3">
+        <v>700059</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" ht="13.5">
+      <c r="A61" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="3">
+        <v>700060</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" ht="13.5">
+      <c r="A62" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" s="3">
+        <v>700061</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" ht="13.5">
+      <c r="A63" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="3">
+        <v>700062</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" ht="13.5">
+      <c r="A64" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C64" s="3">
+        <v>700063</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" ht="13.5">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="3">
+        <v>700064</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" ht="13.5">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="3">
+        <v>700065</v>
+      </c>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:6" ht="13.5">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="3">
+        <v>700066</v>
+      </c>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:6" ht="13.5">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="3">
+        <v>700067</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="1:6" ht="13.5">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="3">
+        <v>700068</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="1:6" ht="13.5">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="3">
+        <v>700069</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="1:6" ht="13.5">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="3">
+        <v>700070</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="1:6" ht="13.5">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="3">
+        <v>700071</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="1:6" ht="13.5">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="3">
+        <v>700072</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="1:6" ht="13.5">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="3">
+        <v>700073</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" spans="1:6" ht="13.5">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="3">
+        <v>700074</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>